<commit_message>
ui modified, credit added
</commit_message>
<xml_diff>
--- a/S_LOGOUT/Assets/Resources/YooJung/ExcelData/game/game_1_2.xlsx
+++ b/S_LOGOUT/Assets/Resources/YooJung/ExcelData/game/game_1_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moon/Downloads/S_LOGOUTf/Assets/Resources/YooJung/ExcelData/game/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moon/Downloads/Proj/Assets/Resources/YooJung/ExcelData/game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A4A93F-AE8C-0F43-A234-785C6519D878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8D369C-2B63-C746-9196-F8340AD1BA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="2200" windowWidth="28300" windowHeight="17440" xr2:uid="{3A795709-8B33-A84B-BFDB-1874F2F0F538}"/>
+    <workbookView xWindow="17920" yWindow="500" windowWidth="17920" windowHeight="21900" xr2:uid="{3A795709-8B33-A84B-BFDB-1874F2F0F538}"/>
   </bookViews>
   <sheets>
     <sheet name="g_1_2" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>index</t>
   </si>
@@ -52,27 +52,12 @@
   </si>
   <si>
     <t>갑자기 공부하는 척? 실망이야 우리 같은 겜망인생인줄 알았는데</t>
-  </si>
-  <si>
-    <t>공부해야지 우리 고1이다 임마</t>
   </si>
   <si>
     <t>네 확인이요 제가 잡을게요^^</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>네 치킨 꼭 드시고요 응원할게요^^</t>
-  </si>
-  <si>
-    <t>그럼 님도 잡을 수 있어요?</t>
-  </si>
-  <si>
-    <t>네? 나를 왜 잡아요ㅋㅋㅋ</t>
-  </si>
-  <si>
-    <t>몰라요 님하고 치킨 뜯게요</t>
-  </si>
-  <si>
     <t>ㅋㅋ그래서 이제 공부하러 감?</t>
   </si>
   <si>
@@ -86,37 +71,12 @@
   </si>
   <si>
     <t>아 금방 감 이번 판만 하고 갈게</t>
-  </si>
-  <si>
-    <t>가끔 핵나오면 짜증나기는 한데 카배도 비슷하니까</t>
-  </si>
-  <si>
-    <t>스킨 많은 건 좋아 뚫어준 애가 솔로 랭커라서 나도 랭크인 해보고 싶은데 어려워.. 솔쿼드 가려면 한참 걸릴듯</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>아 그 친구가 랭커였어? 미쳤다 뭐하는 사람이야ㅋㅋ</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>인생을 게임에 반납했달까ㅋㅋ 그래서 게이머에 인맥 좀 있음</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>오…글쿤</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>외국인들하고는 안해봤어 그럼?</t>
-  </si>
-  <si>
-    <t>한번 했다가 소통 아예 안돼서 솔로로 전향한거ㅋㅋㅋ</t>
-  </si>
-  <si>
-    <t>아하ㅋㅋㅋ</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>너 같이 하면 안돼? 같이 듀쿼드 하면서 솔로 플레이 늘리면 좋을 거 같은데</t>
   </si>
   <si>
@@ -136,22 +96,10 @@
     <t>dkfjskfjl.zip</t>
   </si>
   <si>
-    <t>개인정보 신경쓰이면 안알려줘도 돼 이거 설치해도 스팀배그 가능</t>
-  </si>
-  <si>
-    <t>크랙이라 안알려주려고 했는데 너니까 알려준다</t>
-  </si>
-  <si>
-    <t>아무것도 안 뜨는데?</t>
-  </si>
-  <si>
     <t>ㅎ선물</t>
   </si>
   <si>
     <t>뭐임 이거</t>
-  </si>
-  <si>
-    <t>영통 받아봐</t>
   </si>
   <si>
     <t>안 받아? 딱 두번 더 기회줄게</t>
@@ -177,6 +125,26 @@
   <si>
     <t>계정 뚫으니까 좋음?</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>개인정보 신경쓰이면 안알려줘도 돼 이거 설치해도 게임 가능</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>불법파일이라 안알려주려고 했는데 너니까 알려준다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>가끔 핵나오면 짜증나기는 한데 다른 것도 비슷하니까</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>공부해야지 우리 학생이다 임마</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>합성사진 ㅋㅋ 영통 받아봐</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -600,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2235986-AA0B-4448-ACE5-747C9329FED1}">
   <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -633,10 +601,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="str">
-        <f t="shared" ref="D2:D41" si="0">IF(B2=FALSE,"타인","나")</f>
+        <f t="shared" ref="D2:D33" si="0">IF(B2=FALSE,"타인","나")</f>
         <v>나</v>
       </c>
     </row>
@@ -663,7 +631,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -678,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -693,10 +661,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B6=FALSE,"타인","나")</f>
         <v>나</v>
       </c>
     </row>
@@ -708,10 +676,10 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B7=FALSE,"타인","나")</f>
         <v>타인</v>
       </c>
     </row>
@@ -723,10 +691,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B8=FALSE,"타인","나")</f>
         <v>나</v>
       </c>
     </row>
@@ -734,60 +702,60 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="b">
-        <v>0</v>
+      <c r="B9" t="b">
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>타인</v>
+        <f>IF(B9=FALSE,"타인","나")</f>
+        <v>나</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="b">
-        <v>1</v>
+      <c r="B10" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>나</v>
+        <f>IF(B10=FALSE,"타인","나")</f>
+        <v>타인</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="b">
-        <v>0</v>
+      <c r="B11" t="b">
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>타인</v>
+        <f>IF(B11=FALSE,"타인","나")</f>
+        <v>나</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="b">
-        <v>1</v>
+      <c r="B12" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>나</v>
+        <f>IF(B12=FALSE,"타인","나")</f>
+        <v>타인</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -798,10 +766,10 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B13=FALSE,"타인","나")</f>
         <v>나</v>
       </c>
     </row>
@@ -813,10 +781,10 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D14" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B14=FALSE,"타인","나")</f>
         <v>타인</v>
       </c>
     </row>
@@ -828,10 +796,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D15" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B15=FALSE,"타인","나")</f>
         <v>나</v>
       </c>
     </row>
@@ -843,10 +811,10 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D16" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B16=FALSE,"타인","나")</f>
         <v>타인</v>
       </c>
     </row>
@@ -858,10 +826,10 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D17" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B17=FALSE,"타인","나")</f>
         <v>나</v>
       </c>
     </row>
@@ -873,10 +841,10 @@
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D18" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B18=FALSE,"타인","나")</f>
         <v>타인</v>
       </c>
     </row>
@@ -888,10 +856,10 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D19" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B19=FALSE,"타인","나")</f>
         <v>타인</v>
       </c>
     </row>
@@ -903,10 +871,10 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D20" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B20=FALSE,"타인","나")</f>
         <v>나</v>
       </c>
     </row>
@@ -918,10 +886,10 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D21" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B21=FALSE,"타인","나")</f>
         <v>타인</v>
       </c>
     </row>
@@ -929,30 +897,30 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="b">
-        <v>1</v>
+      <c r="B22" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>나</v>
+        <f>IF(B22=FALSE,"타인","나")</f>
+        <v>타인</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="b">
-        <v>1</v>
+      <c r="B23" s="5" t="b">
+        <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D23" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>나</v>
+        <f>IF(B23=FALSE,"타인","나")</f>
+        <v>타인</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -962,11 +930,11 @@
       <c r="B24" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="C24" t="s">
-        <v>23</v>
+      <c r="C24" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="D24" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D24:D30" si="1">IF(B24=FALSE,"타인","나")</f>
         <v>타인</v>
       </c>
     </row>
@@ -974,14 +942,14 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="b">
+      <c r="B25" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C25" t="s">
-        <v>24</v>
+      <c r="C25" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="D25" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>나</v>
       </c>
     </row>
@@ -992,11 +960,11 @@
       <c r="B26" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="C26" t="s">
-        <v>25</v>
+      <c r="C26" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="D26" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>타인</v>
       </c>
     </row>
@@ -1004,15 +972,15 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" t="b">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>26</v>
+      <c r="B27" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="D27" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>나</v>
+        <f t="shared" si="1"/>
+        <v>타인</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1022,11 +990,11 @@
       <c r="B28" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="C28" t="s">
-        <v>27</v>
+      <c r="C28" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="D28" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>타인</v>
       </c>
     </row>
@@ -1037,11 +1005,11 @@
       <c r="B29" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="C29" t="s">
-        <v>28</v>
+      <c r="C29" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="D29" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>타인</v>
       </c>
     </row>
@@ -1049,208 +1017,76 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="b">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>29</v>
+      <c r="B30" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="D30" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>나</v>
+        <f t="shared" si="1"/>
+        <v>타인</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>타인</v>
-      </c>
+      <c r="A31"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>타인</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>타인</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>나</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="B35" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>타인</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>나</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>타인</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>타인</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-      <c r="B39" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D39" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>타인</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-      <c r="B40" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D40" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>타인</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="1">
-        <v>40</v>
-      </c>
-      <c r="B41" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D41" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>타인</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="A32"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="1"/>
       <c r="B42" s="5"/>
       <c r="C42" s="6"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
     </row>

</xml_diff>